<commit_message>
Translation of Takeoff module + wing_area loop
Takeoff module : remain link to engine (also to be used in cruise)
</commit_message>
<xml_diff>
--- a/modules_breakdown.xlsx
+++ b/modules_breakdown.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="184">
   <si>
     <t>Location</t>
   </si>
@@ -547,6 +547,43 @@
   </si>
   <si>
     <t>removed: not used, only for print</t>
+  </si>
+  <si>
+    <t>GA_wing_sizing.py</t>
+  </si>
+  <si>
+    <t>..\models\loops</t>
+  </si>
+  <si>
+    <t>compute_wing_area.py</t>
+  </si>
+  <si>
+    <t>GA_takeoff.py</t>
+  </si>
+  <si>
+    <t>V2</t>
+  </si>
+  <si>
+    <t>..\models\aerodynamics\performances</t>
+  </si>
+  <si>
+    <t>simulate_takeoff.py</t>
+  </si>
+  <si>
+    <t>_v2</t>
+  </si>
+  <si>
+    <t>VR</t>
+  </si>
+  <si>
+    <t>_vloff
+_vr</t>
+  </si>
+  <si>
+    <t>takeoff_speeds</t>
+  </si>
+  <si>
+    <t>takeoff_AEO</t>
   </si>
 </sst>
 </file>
@@ -610,9 +647,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -628,6 +662,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -933,10 +970,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:H73"/>
+  <dimension ref="A2:H78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C73" sqref="C73"/>
+    <sheetView tabSelected="1" topLeftCell="B60" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C77" sqref="C77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -987,11 +1024,11 @@
       <c r="E3" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -1121,11 +1158,11 @@
       <c r="E9" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="F9" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -1163,11 +1200,11 @@
       <c r="E11" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="F11" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -1205,11 +1242,11 @@
       <c r="E13" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F13" s="5" t="s">
+      <c r="F13" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -1293,11 +1330,11 @@
       <c r="E17" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F17" s="5" t="s">
+      <c r="F17" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
@@ -1312,11 +1349,11 @@
       <c r="E18" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F18" s="5" t="s">
+      <c r="F18" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="12"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
@@ -1331,11 +1368,11 @@
       <c r="E19" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F19" s="5" t="s">
+      <c r="F19" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="12"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
@@ -1350,11 +1387,11 @@
       <c r="E20" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F20" s="5" t="s">
+      <c r="F20" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
@@ -1392,11 +1429,11 @@
       <c r="E22" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F22" s="5" t="s">
+      <c r="F22" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="G22" s="5"/>
-      <c r="H22" s="5"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="12"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
@@ -1411,11 +1448,11 @@
       <c r="E23" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F23" s="5" t="s">
+      <c r="F23" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="G23" s="5"/>
-      <c r="H23" s="5"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="12"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
@@ -1430,11 +1467,11 @@
       <c r="E24" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F24" s="5" t="s">
+      <c r="F24" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="G24" s="5"/>
-      <c r="H24" s="5"/>
+      <c r="G24" s="12"/>
+      <c r="H24" s="12"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
@@ -1449,11 +1486,11 @@
       <c r="E25" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F25" s="5" t="s">
+      <c r="F25" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="G25" s="5"/>
-      <c r="H25" s="5"/>
+      <c r="G25" s="12"/>
+      <c r="H25" s="12"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
@@ -1494,11 +1531,11 @@
       <c r="E27" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F27" s="5" t="s">
+      <c r="F27" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="G27" s="5"/>
-      <c r="H27" s="5"/>
+      <c r="G27" s="12"/>
+      <c r="H27" s="12"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
@@ -1568,11 +1605,11 @@
       <c r="E30" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F30" s="5" t="s">
+      <c r="F30" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="G30" s="5"/>
-      <c r="H30" s="5"/>
+      <c r="G30" s="12"/>
+      <c r="H30" s="12"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
@@ -1613,11 +1650,11 @@
       <c r="E32" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F32" s="5" t="s">
+      <c r="F32" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="G32" s="5"/>
-      <c r="H32" s="5"/>
+      <c r="G32" s="12"/>
+      <c r="H32" s="12"/>
     </row>
     <row r="33" spans="1:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
@@ -1685,11 +1722,11 @@
       <c r="E35" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F35" s="5" t="s">
+      <c r="F35" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="G35" s="5"/>
-      <c r="H35" s="5"/>
+      <c r="G35" s="12"/>
+      <c r="H35" s="12"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
@@ -2161,11 +2198,11 @@
       <c r="E56" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F56" s="5" t="s">
+      <c r="F56" s="12" t="s">
         <v>129</v>
       </c>
-      <c r="G56" s="5"/>
-      <c r="H56" s="5"/>
+      <c r="G56" s="12"/>
+      <c r="H56" s="12"/>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
@@ -2209,7 +2246,7 @@
       <c r="F58" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="G58" s="6" t="s">
+      <c r="G58" s="5" t="s">
         <v>136</v>
       </c>
     </row>
@@ -2295,7 +2332,7 @@
       <c r="F62" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="G62" s="6" t="s">
+      <c r="G62" s="5" t="s">
         <v>155</v>
       </c>
     </row>
@@ -2312,11 +2349,11 @@
       <c r="E63" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F63" s="5" t="s">
+      <c r="F63" s="12" t="s">
         <v>129</v>
       </c>
-      <c r="G63" s="5"/>
-      <c r="H63" s="5"/>
+      <c r="G63" s="12"/>
+      <c r="H63" s="12"/>
     </row>
     <row r="64" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
@@ -2335,21 +2372,21 @@
       <c r="F64" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="G64" s="6" t="s">
+      <c r="G64" s="5" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="65" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B65" s="7" t="s">
+    <row r="65" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B65" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="C65" s="8" t="s">
+      <c r="C65" s="7" t="s">
         <v>160</v>
       </c>
-      <c r="E65" s="9" t="s">
+      <c r="E65" s="8" t="s">
         <v>27</v>
       </c>
     </row>
@@ -2360,7 +2397,7 @@
       <c r="B66" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C66" s="6" t="s">
+      <c r="C66" s="5" t="s">
         <v>162</v>
       </c>
       <c r="E66" s="3" t="s">
@@ -2372,91 +2409,91 @@
       <c r="G66" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="H66" s="6" t="s">
+      <c r="H66" s="5" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="67" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B67" s="7" t="s">
+    <row r="67" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B67" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="C67" s="8" t="s">
+      <c r="C67" s="7" t="s">
         <v>164</v>
       </c>
-      <c r="E67" s="9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B68" s="7" t="s">
+      <c r="E67" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B68" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="C68" s="8" t="s">
+      <c r="C68" s="7" t="s">
         <v>165</v>
       </c>
-      <c r="E68" s="9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B69" s="7" t="s">
+      <c r="E68" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B69" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="C69" s="8" t="s">
+      <c r="C69" s="7" t="s">
         <v>166</v>
       </c>
-      <c r="E69" s="9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B70" s="7" t="s">
+      <c r="E69" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B70" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="C70" s="8" t="s">
+      <c r="C70" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="E70" s="9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="71" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B71" s="7" t="s">
+      <c r="E70" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B71" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="C71" s="8" t="s">
+      <c r="C71" s="7" t="s">
         <v>168</v>
       </c>
-      <c r="E71" s="9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="72" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B72" s="10" t="s">
+      <c r="E71" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B72" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="C72" s="11" t="s">
+      <c r="C72" s="10" t="s">
         <v>169</v>
       </c>
-      <c r="E72" s="12" t="s">
+      <c r="E72" s="11" t="s">
         <v>27</v>
       </c>
       <c r="F72" s="13" t="s">
@@ -2465,17 +2502,17 @@
       <c r="G72" s="13"/>
       <c r="H72" s="13"/>
     </row>
-    <row r="73" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B73" s="10" t="s">
+    <row r="73" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B73" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="C73" s="11" t="s">
+      <c r="C73" s="10" t="s">
         <v>170</v>
       </c>
-      <c r="E73" s="12" t="s">
+      <c r="E73" s="11" t="s">
         <v>27</v>
       </c>
       <c r="F73" s="13" t="s">
@@ -2484,23 +2521,103 @@
       <c r="G73" s="13"/>
       <c r="H73" s="13"/>
     </row>
+    <row r="74" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B74" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="E74" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="F74" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="G74" s="10" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A75" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B75" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="C75" t="s">
+        <v>176</v>
+      </c>
+      <c r="E75" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="F75" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="G75" t="s">
+        <v>178</v>
+      </c>
+      <c r="H75" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A76" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B76" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="D76" s="2"/>
+      <c r="E76" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="F76" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="G76" t="s">
+        <v>178</v>
+      </c>
+      <c r="H76" s="5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B77" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B78" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>183</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="F3:H3"/>
+    <mergeCell ref="F9:H9"/>
+    <mergeCell ref="F11:H11"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="F17:H17"/>
+    <mergeCell ref="F18:H18"/>
+    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="F20:H20"/>
+    <mergeCell ref="F22:H22"/>
+    <mergeCell ref="F23:H23"/>
     <mergeCell ref="F24:H24"/>
     <mergeCell ref="F56:H56"/>
     <mergeCell ref="F63:H63"/>
     <mergeCell ref="F72:H72"/>
     <mergeCell ref="F73:H73"/>
-    <mergeCell ref="F18:H18"/>
-    <mergeCell ref="F19:H19"/>
-    <mergeCell ref="F20:H20"/>
-    <mergeCell ref="F22:H22"/>
-    <mergeCell ref="F23:H23"/>
-    <mergeCell ref="F3:H3"/>
-    <mergeCell ref="F9:H9"/>
-    <mergeCell ref="F11:H11"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="F17:H17"/>
     <mergeCell ref="F27:H27"/>
     <mergeCell ref="F30:H30"/>
     <mergeCell ref="F32:H32"/>

</xml_diff>

<commit_message>
Update after massbreakdown+geometry pytest success
</commit_message>
<xml_diff>
--- a/modules_breakdown.xlsx
+++ b/modules_breakdown.xlsx
@@ -9,14 +9,17 @@
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
     <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
-    <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Feuil1!$A$1:$H$1</definedName>
+  </definedNames>
   <calcPr calcId="145621"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="186">
   <si>
     <t>Location</t>
   </si>
@@ -67,9 +70,6 @@
   </si>
   <si>
     <t>EmpenageWeight</t>
-  </si>
-  <si>
-    <t>Not used: removed</t>
   </si>
   <si>
     <t>compute_flight_controls_weight</t>
@@ -406,9 +406,6 @@
   </si>
   <si>
     <t>stability_long</t>
-  </si>
-  <si>
-    <t>removed: not used</t>
   </si>
   <si>
     <t>clalpha_wing_cruise</t>
@@ -546,9 +543,6 @@
     <t>maximum_LD</t>
   </si>
   <si>
-    <t>removed: not used, only for print</t>
-  </si>
-  <si>
     <t>GA_wing_sizing.py</t>
   </si>
   <si>
@@ -565,9 +559,6 @@
   </si>
   <si>
     <t>..\models\aerodynamics\performances</t>
-  </si>
-  <si>
-    <t>simulate_takeoff.py</t>
   </si>
   <si>
     <t>_v2</t>
@@ -584,6 +575,24 @@
   </si>
   <si>
     <t>takeoff_AEO</t>
+  </si>
+  <si>
+    <t>Removed: not used</t>
+  </si>
+  <si>
+    <t>Removed: not used, only for print</t>
+  </si>
+  <si>
+    <t>takeoff_BFL</t>
+  </si>
+  <si>
+    <t>takeoff.py</t>
+  </si>
+  <si>
+    <t>TakeOffSpeed</t>
+  </si>
+  <si>
+    <t>TakeOffPhase</t>
   </si>
 </sst>
 </file>
@@ -606,7 +615,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -616,6 +625,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -632,7 +659,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -666,7 +693,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -970,10 +999,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:H78"/>
+  <dimension ref="A1:H78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B60" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C77" sqref="C77"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A79" sqref="A79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -986,30 +1015,51 @@
     <col min="6" max="6" width="55" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="36.140625" customWidth="1"/>
     <col min="8" max="8" width="36.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="11.42578125" style="14"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>67</v>
+      </c>
+    </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" t="s">
-        <v>0</v>
-      </c>
-      <c r="G2" t="s">
-        <v>2</v>
-      </c>
-      <c r="H2" t="s">
-        <v>68</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>180</v>
+      </c>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -1019,16 +1069,20 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F3" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12"/>
+        <v>26</v>
+      </c>
+      <c r="F3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -1038,19 +1092,19 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F4" t="s">
         <v>14</v>
       </c>
       <c r="G4" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="H4" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -1061,19 +1115,19 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F5" t="s">
         <v>14</v>
       </c>
       <c r="G5" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="H5" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -1084,19 +1138,19 @@
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F6" t="s">
         <v>14</v>
       </c>
       <c r="G6" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="H6" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -1107,19 +1161,19 @@
         <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F7" t="s">
         <v>14</v>
       </c>
       <c r="G7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7" t="s">
         <v>21</v>
-      </c>
-      <c r="H7" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -1133,17 +1187,13 @@
         <v>23</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F8" t="s">
-        <v>14</v>
-      </c>
-      <c r="G8" t="s">
-        <v>20</v>
-      </c>
-      <c r="H8" t="s">
-        <v>22</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="F8" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -1153,16 +1203,20 @@
         <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F9" t="s">
         <v>27</v>
       </c>
-      <c r="F9" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
+      <c r="G9" t="s">
+        <v>28</v>
+      </c>
+      <c r="H9" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -1172,20 +1226,16 @@
         <v>3</v>
       </c>
       <c r="C10" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F10" t="s">
-        <v>28</v>
-      </c>
-      <c r="G10" t="s">
-        <v>29</v>
-      </c>
-      <c r="H10" t="s">
-        <v>30</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="F10" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -1195,16 +1245,20 @@
         <v>3</v>
       </c>
       <c r="C11" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F11" t="s">
         <v>27</v>
       </c>
-      <c r="F11" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
+      <c r="G11" t="s">
+        <v>30</v>
+      </c>
+      <c r="H11" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -1214,20 +1268,16 @@
         <v>3</v>
       </c>
       <c r="C12" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F12" t="s">
-        <v>28</v>
-      </c>
-      <c r="G12" t="s">
-        <v>31</v>
-      </c>
-      <c r="H12" t="s">
-        <v>32</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="F12" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -1240,13 +1290,17 @@
         <v>35</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F13" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
+        <v>26</v>
+      </c>
+      <c r="F13" t="s">
+        <v>37</v>
+      </c>
+      <c r="G13" t="s">
+        <v>36</v>
+      </c>
+      <c r="H13" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -1256,16 +1310,16 @@
         <v>3</v>
       </c>
       <c r="C14" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F14" t="s">
+        <v>37</v>
+      </c>
+      <c r="G14" t="s">
         <v>38</v>
-      </c>
-      <c r="G14" t="s">
-        <v>37</v>
       </c>
       <c r="H14" t="s">
         <v>40</v>
@@ -1282,16 +1336,16 @@
         <v>44</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G15" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="H15" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -1305,17 +1359,13 @@
         <v>45</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F16" t="s">
-        <v>38</v>
-      </c>
-      <c r="G16" t="s">
-        <v>42</v>
-      </c>
-      <c r="H16" t="s">
-        <v>43</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="F16" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="G16" s="15"/>
+      <c r="H16" s="15"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
@@ -1328,13 +1378,13 @@
         <v>46</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F17" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="G17" s="12"/>
-      <c r="H17" s="12"/>
+        <v>26</v>
+      </c>
+      <c r="F17" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="G17" s="15"/>
+      <c r="H17" s="15"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
@@ -1347,13 +1397,13 @@
         <v>47</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F18" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="G18" s="12"/>
-      <c r="H18" s="12"/>
+        <v>26</v>
+      </c>
+      <c r="F18" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="G18" s="15"/>
+      <c r="H18" s="15"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
@@ -1366,13 +1416,13 @@
         <v>48</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F19" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="G19" s="12"/>
-      <c r="H19" s="12"/>
+        <v>26</v>
+      </c>
+      <c r="F19" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="G19" s="15"/>
+      <c r="H19" s="15"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
@@ -1385,13 +1435,17 @@
         <v>49</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F20" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="G20" s="12"/>
-      <c r="H20" s="12"/>
+        <v>26</v>
+      </c>
+      <c r="F20" t="s">
+        <v>50</v>
+      </c>
+      <c r="G20" t="s">
+        <v>51</v>
+      </c>
+      <c r="H20" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
@@ -1401,20 +1455,16 @@
         <v>3</v>
       </c>
       <c r="C21" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F21" t="s">
-        <v>51</v>
-      </c>
-      <c r="G21" t="s">
-        <v>52</v>
-      </c>
-      <c r="H21" t="s">
-        <v>53</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="F21" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="G21" s="15"/>
+      <c r="H21" s="15"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
@@ -1427,13 +1477,13 @@
         <v>54</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F22" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="G22" s="12"/>
-      <c r="H22" s="12"/>
+        <v>26</v>
+      </c>
+      <c r="F22" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="G22" s="15"/>
+      <c r="H22" s="15"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
@@ -1446,13 +1496,13 @@
         <v>55</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F23" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="G23" s="12"/>
-      <c r="H23" s="12"/>
+        <v>26</v>
+      </c>
+      <c r="F23" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="G23" s="15"/>
+      <c r="H23" s="15"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
@@ -1465,13 +1515,13 @@
         <v>56</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F24" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="G24" s="12"/>
-      <c r="H24" s="12"/>
+        <v>26</v>
+      </c>
+      <c r="F24" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="G24" s="15"/>
+      <c r="H24" s="15"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
@@ -1484,83 +1534,90 @@
         <v>57</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F25" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="G25" s="12"/>
-      <c r="H25" s="12"/>
+        <v>26</v>
+      </c>
+      <c r="F25" t="s">
+        <v>59</v>
+      </c>
+      <c r="G25" t="s">
+        <v>58</v>
+      </c>
+      <c r="H25" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>1</v>
       </c>
       <c r="B26" t="s">
-        <v>3</v>
+        <v>77</v>
       </c>
       <c r="C26" t="s">
-        <v>58</v>
+        <v>78</v>
+      </c>
+      <c r="D26" t="s">
+        <v>79</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F26" t="s">
-        <v>60</v>
-      </c>
-      <c r="G26" t="s">
-        <v>59</v>
-      </c>
-      <c r="H26" t="s">
-        <v>61</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="F26" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="G26" s="12"/>
+      <c r="H26" s="12"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>1</v>
       </c>
       <c r="B27" t="s">
+        <v>77</v>
+      </c>
+      <c r="C27" t="s">
         <v>78</v>
       </c>
-      <c r="C27" t="s">
-        <v>79</v>
-      </c>
       <c r="D27" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F27" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="G27" s="12"/>
-      <c r="H27" s="12"/>
+        <v>26</v>
+      </c>
+      <c r="F27" t="s">
+        <v>82</v>
+      </c>
+      <c r="G27" t="s">
+        <v>83</v>
+      </c>
+      <c r="H27" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>1</v>
       </c>
       <c r="B28" t="s">
+        <v>77</v>
+      </c>
+      <c r="C28" t="s">
         <v>78</v>
       </c>
-      <c r="C28" t="s">
-        <v>79</v>
-      </c>
       <c r="D28" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F28" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="G28" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="H28" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -1568,187 +1625,184 @@
         <v>1</v>
       </c>
       <c r="B29" t="s">
+        <v>77</v>
+      </c>
+      <c r="C29" t="s">
         <v>78</v>
       </c>
-      <c r="C29" t="s">
-        <v>79</v>
-      </c>
       <c r="D29" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F29" t="s">
-        <v>87</v>
-      </c>
-      <c r="G29" t="s">
-        <v>88</v>
-      </c>
-      <c r="H29" t="s">
-        <v>88</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="F29" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="G29" s="15"/>
+      <c r="H29" s="15"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>1</v>
       </c>
       <c r="B30" t="s">
+        <v>77</v>
+      </c>
+      <c r="C30" t="s">
         <v>78</v>
       </c>
-      <c r="C30" t="s">
-        <v>79</v>
-      </c>
       <c r="D30" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F30" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="G30" s="12"/>
-      <c r="H30" s="12"/>
+        <v>26</v>
+      </c>
+      <c r="F30" t="s">
+        <v>86</v>
+      </c>
+      <c r="G30" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>1</v>
       </c>
       <c r="B31" t="s">
+        <v>77</v>
+      </c>
+      <c r="C31" t="s">
         <v>78</v>
       </c>
-      <c r="C31" t="s">
-        <v>79</v>
-      </c>
       <c r="D31" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F31" t="s">
-        <v>87</v>
-      </c>
-      <c r="G31" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>1</v>
-      </c>
-      <c r="B32" t="s">
+        <v>26</v>
+      </c>
+      <c r="F31" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="G31" s="12"/>
+      <c r="H31" s="12"/>
+    </row>
+    <row r="32" spans="1:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C32" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="C32" t="s">
-        <v>79</v>
-      </c>
-      <c r="D32" t="s">
-        <v>93</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F32" s="12" t="s">
+      <c r="D32" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="G32" s="12"/>
-      <c r="H32" s="12"/>
-    </row>
-    <row r="33" spans="1:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B33" s="2" t="s">
+      <c r="E32" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="G32" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="H32" s="2"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>1</v>
+      </c>
+      <c r="B33" t="s">
+        <v>77</v>
+      </c>
+      <c r="C33" t="s">
         <v>78</v>
       </c>
-      <c r="C33" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>95</v>
+      <c r="D33" t="s">
+        <v>97</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F33" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="G33" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="H33" s="2"/>
+        <v>26</v>
+      </c>
+      <c r="F33" t="s">
+        <v>82</v>
+      </c>
+      <c r="G33" t="s">
+        <v>83</v>
+      </c>
+      <c r="H33" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>1</v>
       </c>
       <c r="B34" t="s">
+        <v>77</v>
+      </c>
+      <c r="C34" t="s">
         <v>78</v>
-      </c>
-      <c r="C34" t="s">
-        <v>79</v>
       </c>
       <c r="D34" t="s">
         <v>98</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F34" t="s">
-        <v>83</v>
-      </c>
-      <c r="G34" t="s">
-        <v>84</v>
-      </c>
-      <c r="H34" t="s">
-        <v>85</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="F34" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="G34" s="15"/>
+      <c r="H34" s="15"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>1</v>
       </c>
       <c r="B35" t="s">
+        <v>77</v>
+      </c>
+      <c r="C35" t="s">
         <v>78</v>
-      </c>
-      <c r="C35" t="s">
-        <v>79</v>
       </c>
       <c r="D35" t="s">
         <v>99</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F35" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="G35" s="12"/>
-      <c r="H35" s="12"/>
+        <v>26</v>
+      </c>
+      <c r="F35" t="s">
+        <v>100</v>
+      </c>
+      <c r="G35" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>1</v>
       </c>
       <c r="B36" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C36" t="s">
-        <v>79</v>
-      </c>
-      <c r="D36" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F36" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="G36" t="s">
-        <v>102</v>
+        <v>106</v>
+      </c>
+      <c r="H36" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
@@ -1756,22 +1810,19 @@
         <v>1</v>
       </c>
       <c r="B37" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C37" t="s">
+        <v>104</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F37" t="s">
         <v>103</v>
       </c>
-      <c r="E37" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F37" t="s">
-        <v>106</v>
-      </c>
       <c r="G37" t="s">
-        <v>107</v>
-      </c>
-      <c r="H37" t="s">
-        <v>108</v>
+        <v>87</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
@@ -1779,19 +1830,19 @@
         <v>1</v>
       </c>
       <c r="B38" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C38" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F38" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="G38" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
@@ -1799,19 +1850,19 @@
         <v>1</v>
       </c>
       <c r="B39" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C39" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F39" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="G39" t="s">
-        <v>88</v>
+        <v>112</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
@@ -1819,19 +1870,19 @@
         <v>1</v>
       </c>
       <c r="B40" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C40" t="s">
+        <v>113</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F40" t="s">
         <v>111</v>
       </c>
-      <c r="E40" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F40" t="s">
-        <v>112</v>
-      </c>
       <c r="G40" t="s">
-        <v>113</v>
+        <v>87</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
@@ -1839,19 +1890,22 @@
         <v>1</v>
       </c>
       <c r="B41" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C41" t="s">
         <v>114</v>
       </c>
+      <c r="D41" t="s">
+        <v>115</v>
+      </c>
       <c r="E41" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F41" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G41" t="s">
-        <v>88</v>
+        <v>116</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
@@ -1859,22 +1913,19 @@
         <v>1</v>
       </c>
       <c r="B42" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C42" t="s">
-        <v>115</v>
-      </c>
-      <c r="D42" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F42" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="G42" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
@@ -1882,19 +1933,19 @@
         <v>1</v>
       </c>
       <c r="B43" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C43" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F43" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="G43" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
@@ -1902,19 +1953,19 @@
         <v>1</v>
       </c>
       <c r="B44" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C44" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F44" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="G44" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
@@ -1922,19 +1973,19 @@
         <v>1</v>
       </c>
       <c r="B45" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C45" t="s">
+        <v>125</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F45" t="s">
         <v>123</v>
       </c>
-      <c r="E45" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F45" t="s">
-        <v>124</v>
-      </c>
       <c r="G45" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
@@ -1942,19 +1993,25 @@
         <v>1</v>
       </c>
       <c r="B46" t="s">
-        <v>78</v>
+        <v>62</v>
       </c>
       <c r="C46" t="s">
-        <v>126</v>
-      </c>
-      <c r="E46" s="3" t="s">
-        <v>27</v>
+        <v>61</v>
+      </c>
+      <c r="D46" t="s">
+        <v>63</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="F46" t="s">
-        <v>124</v>
+        <v>64</v>
       </c>
       <c r="G46" t="s">
-        <v>127</v>
+        <v>65</v>
+      </c>
+      <c r="H46" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
@@ -1962,25 +2019,25 @@
         <v>1</v>
       </c>
       <c r="B47" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C47" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D47" t="s">
+        <v>68</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F47" t="s">
         <v>64</v>
       </c>
-      <c r="E47" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F47" t="s">
-        <v>65</v>
-      </c>
       <c r="G47" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="H47" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
@@ -1988,25 +2045,25 @@
         <v>1</v>
       </c>
       <c r="B48" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C48" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D48" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F48" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G48" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="H48" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
@@ -2014,25 +2071,25 @@
         <v>1</v>
       </c>
       <c r="B49" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C49" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D49" t="s">
         <v>72</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F49" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G49" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="H49" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
@@ -2040,25 +2097,25 @@
         <v>1</v>
       </c>
       <c r="B50" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C50" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D50" t="s">
-        <v>73</v>
+        <v>139</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F50" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G50" t="s">
-        <v>76</v>
+        <v>140</v>
       </c>
       <c r="H50" t="s">
-        <v>77</v>
+        <v>141</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
@@ -2066,25 +2123,25 @@
         <v>1</v>
       </c>
       <c r="B51" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C51" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D51" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F51" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G51" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="H51" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
@@ -2092,25 +2149,25 @@
         <v>1</v>
       </c>
       <c r="B52" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C52" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D52" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F52" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G52" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="H52" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
@@ -2118,19 +2175,16 @@
         <v>1</v>
       </c>
       <c r="B53" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C53" t="s">
-        <v>62</v>
-      </c>
-      <c r="D53" t="s">
-        <v>147</v>
+        <v>61</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F53" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G53" t="s">
         <v>148</v>
@@ -2144,22 +2198,22 @@
         <v>1</v>
       </c>
       <c r="B54" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C54" t="s">
-        <v>62</v>
+        <v>150</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F54" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G54" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="H54" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
@@ -2167,86 +2221,83 @@
         <v>1</v>
       </c>
       <c r="B55" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C55" t="s">
-        <v>152</v>
+        <v>127</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F55" t="s">
-        <v>65</v>
-      </c>
-      <c r="G55" t="s">
-        <v>142</v>
-      </c>
-      <c r="H55" t="s">
-        <v>143</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="F55" s="15" t="s">
+        <v>180</v>
+      </c>
+      <c r="G55" s="15"/>
+      <c r="H55" s="15"/>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>1</v>
       </c>
       <c r="B56" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C56" t="s">
         <v>128</v>
       </c>
+      <c r="D56" t="s">
+        <v>129</v>
+      </c>
       <c r="E56" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F56" s="12" t="s">
-        <v>129</v>
-      </c>
-      <c r="G56" s="12"/>
-      <c r="H56" s="12"/>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>1</v>
-      </c>
-      <c r="B57" t="s">
-        <v>63</v>
-      </c>
-      <c r="C57" t="s">
+        <v>26</v>
+      </c>
+      <c r="F56" t="s">
         <v>130</v>
       </c>
-      <c r="D57" t="s">
+      <c r="G56" t="s">
         <v>131</v>
       </c>
-      <c r="E57" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F57" t="s">
+    </row>
+    <row r="57" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A57" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="D57" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="G57" t="s">
+      <c r="E57" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F57" s="2" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="58" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="G57" s="5" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C58" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C58" t="s">
+        <v>135</v>
+      </c>
+      <c r="E58" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F58" t="s">
         <v>130</v>
       </c>
-      <c r="D58" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="E58" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F58" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="G58" s="5" t="s">
+      <c r="G58" t="s">
         <v>136</v>
       </c>
     </row>
@@ -2255,16 +2306,16 @@
         <v>1</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C59" t="s">
         <v>137</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F59" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="G59" t="s">
         <v>138</v>
@@ -2275,354 +2326,414 @@
         <v>1</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C60" t="s">
-        <v>139</v>
-      </c>
-      <c r="E60" s="3" t="s">
-        <v>27</v>
+        <v>151</v>
+      </c>
+      <c r="D60" t="s">
+        <v>129</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="F60" t="s">
+        <v>130</v>
+      </c>
+      <c r="G60" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A61" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="D61" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="G60" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A61" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B61" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C61" t="s">
+      <c r="E61" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F61" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="G61" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="D61" t="s">
-        <v>131</v>
-      </c>
-      <c r="E61" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F61" t="s">
-        <v>132</v>
-      </c>
-      <c r="G61" t="s">
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A62" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C62" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="62" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A62" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B62" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C62" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="D62" s="2" t="s">
-        <v>134</v>
-      </c>
       <c r="E62" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F62" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="G62" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F62" s="15" t="s">
+        <v>180</v>
+      </c>
+      <c r="G62" s="15"/>
+      <c r="H62" s="15"/>
+    </row>
+    <row r="63" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A63" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C63" s="2" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A63" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B63" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C63" t="s">
+      <c r="D63" s="2"/>
+      <c r="E63" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F63" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="G63" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="E63" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F63" s="12" t="s">
-        <v>129</v>
-      </c>
-      <c r="G63" s="12"/>
-      <c r="H63" s="12"/>
-    </row>
-    <row r="64" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A64" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B64" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C64" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="D64" s="2"/>
-      <c r="E64" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F64" s="4" t="s">
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A64" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B64" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C64" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="D64" s="7"/>
+      <c r="E64" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="F64" s="7"/>
+      <c r="G64" s="7"/>
+      <c r="H64" s="7"/>
+    </row>
+    <row r="65" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A65" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C65" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="E65" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F65" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="G65" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="G64" s="5" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B65" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="C65" s="7" t="s">
-        <v>160</v>
-      </c>
-      <c r="E65" s="8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A66" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B66" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C66" s="5" t="s">
+      <c r="H65" s="5" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A66" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B66" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C66" s="7" t="s">
         <v>162</v>
       </c>
-      <c r="E66" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F66" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="G66" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="H66" s="5" t="s">
+      <c r="D66" s="7"/>
+      <c r="E66" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="F66" s="7"/>
+      <c r="G66" s="7"/>
+      <c r="H66" s="7"/>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A67" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B67" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C67" s="7" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="67" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B67" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="C67" s="7" t="s">
+      <c r="D67" s="7"/>
+      <c r="E67" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="F67" s="7"/>
+      <c r="G67" s="7"/>
+      <c r="H67" s="7"/>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A68" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B68" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C68" s="7" t="s">
         <v>164</v>
       </c>
-      <c r="E67" s="8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B68" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="C68" s="7" t="s">
+      <c r="D68" s="7"/>
+      <c r="E68" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="F68" s="7"/>
+      <c r="G68" s="7"/>
+      <c r="H68" s="7"/>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A69" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B69" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C69" s="7" t="s">
         <v>165</v>
       </c>
-      <c r="E68" s="8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B69" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="C69" s="7" t="s">
+      <c r="D69" s="7"/>
+      <c r="E69" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="F69" s="7"/>
+      <c r="G69" s="7"/>
+      <c r="H69" s="7"/>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A70" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B70" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C70" s="7" t="s">
         <v>166</v>
       </c>
-      <c r="E69" s="8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B70" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="C70" s="7" t="s">
+      <c r="D70" s="7"/>
+      <c r="E70" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="F70" s="7"/>
+      <c r="G70" s="7"/>
+      <c r="H70" s="7"/>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A71" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B71" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="C71" s="10" t="s">
         <v>167</v>
       </c>
-      <c r="E70" s="8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="71" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B71" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="C71" s="7" t="s">
+      <c r="D71" s="10"/>
+      <c r="E71" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="F71" s="15" t="s">
+        <v>180</v>
+      </c>
+      <c r="G71" s="15"/>
+      <c r="H71" s="15"/>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A72" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B72" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="C72" s="10" t="s">
         <v>168</v>
       </c>
-      <c r="E71" s="8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="72" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="B72" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="C72" s="10" t="s">
+      <c r="D72" s="10"/>
+      <c r="E72" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="F72" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="G72" s="15"/>
+      <c r="H72" s="15"/>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A73" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B73" s="9" t="s">
         <v>169</v>
       </c>
-      <c r="E72" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="F72" s="13" t="s">
-        <v>129</v>
-      </c>
-      <c r="G72" s="13"/>
-      <c r="H72" s="13"/>
-    </row>
-    <row r="73" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="B73" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="C73" s="10" t="s">
+      <c r="C73" s="10"/>
+      <c r="D73" s="10"/>
+      <c r="E73" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="F73" s="10" t="s">
         <v>170</v>
       </c>
-      <c r="E73" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="F73" s="13" t="s">
+      <c r="G73" s="10" t="s">
         <v>171</v>
       </c>
-      <c r="G73" s="13"/>
-      <c r="H73" s="13"/>
-    </row>
-    <row r="74" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H73" s="10"/>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="9" t="s">
         <v>1</v>
       </c>
       <c r="B74" s="9" t="s">
         <v>172</v>
       </c>
+      <c r="C74" t="s">
+        <v>173</v>
+      </c>
       <c r="E74" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="F74" s="10" t="s">
-        <v>173</v>
-      </c>
-      <c r="G74" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="F74" s="2" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G74" t="s">
+        <v>183</v>
+      </c>
+      <c r="H74" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A75" s="9" t="s">
         <v>1</v>
       </c>
       <c r="B75" s="9" t="s">
-        <v>175</v>
-      </c>
-      <c r="C75" t="s">
+        <v>172</v>
+      </c>
+      <c r="C75" s="2" t="s">
         <v>176</v>
       </c>
+      <c r="D75" s="2"/>
       <c r="E75" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F75" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="G75" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="H75" s="5" t="s">
         <v>177</v>
       </c>
-      <c r="G75" t="s">
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A76" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B76" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="C76" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="H75" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="76" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A76" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="B76" s="9" t="s">
-        <v>175</v>
-      </c>
-      <c r="C76" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="D76" s="2"/>
       <c r="E76" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="G76" t="s">
-        <v>178</v>
+        <v>174</v>
+      </c>
+      <c r="G76" s="2" t="s">
+        <v>183</v>
       </c>
       <c r="H76" s="5" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A77" s="9" t="s">
+        <v>1</v>
+      </c>
       <c r="B77" s="9" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C77" s="2" t="s">
         <v>182</v>
       </c>
+      <c r="E77" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="F77" s="15" t="s">
+        <v>180</v>
+      </c>
+      <c r="G77" s="15"/>
+      <c r="H77" s="15"/>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A78" s="9" t="s">
+        <v>1</v>
+      </c>
       <c r="B78" s="9" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C78" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="E78" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="F78" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="G78" s="2" t="s">
         <v>183</v>
       </c>
+      <c r="H78" t="s">
+        <v>185</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="20">
-    <mergeCell ref="F3:H3"/>
-    <mergeCell ref="F9:H9"/>
-    <mergeCell ref="F11:H11"/>
-    <mergeCell ref="F13:H13"/>
+  <autoFilter ref="A1:H1"/>
+  <mergeCells count="21">
+    <mergeCell ref="F77:H77"/>
+    <mergeCell ref="F23:H23"/>
+    <mergeCell ref="F55:H55"/>
+    <mergeCell ref="F62:H62"/>
+    <mergeCell ref="F71:H71"/>
+    <mergeCell ref="F72:H72"/>
+    <mergeCell ref="F26:H26"/>
+    <mergeCell ref="F29:H29"/>
+    <mergeCell ref="F31:H31"/>
+    <mergeCell ref="F34:H34"/>
+    <mergeCell ref="F24:H24"/>
     <mergeCell ref="F17:H17"/>
     <mergeCell ref="F18:H18"/>
     <mergeCell ref="F19:H19"/>
-    <mergeCell ref="F20:H20"/>
+    <mergeCell ref="F21:H21"/>
     <mergeCell ref="F22:H22"/>
-    <mergeCell ref="F23:H23"/>
-    <mergeCell ref="F24:H24"/>
-    <mergeCell ref="F56:H56"/>
-    <mergeCell ref="F63:H63"/>
-    <mergeCell ref="F72:H72"/>
-    <mergeCell ref="F73:H73"/>
-    <mergeCell ref="F27:H27"/>
-    <mergeCell ref="F30:H30"/>
-    <mergeCell ref="F32:H32"/>
-    <mergeCell ref="F35:H35"/>
-    <mergeCell ref="F25:H25"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="F8:H8"/>
+    <mergeCell ref="F10:H10"/>
+    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="F16:H16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2638,16 +2749,4 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Update of mission/takeoff and propulsion
Update before pytests
</commit_message>
<xml_diff>
--- a/modules_breakdown.xlsx
+++ b/modules_breakdown.xlsx
@@ -14,12 +14,11 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Feuil1!$A$1:$H$1</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="185">
   <si>
     <t>Location</t>
   </si>
@@ -91,9 +90,6 @@
   </si>
   <si>
     <t>compute_paint_weight</t>
-  </si>
-  <si>
-    <t>Model removed because equal to constant defined in .xml file</t>
   </si>
   <si>
     <t>compute_engine_weight</t>
@@ -690,12 +686,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1001,8 +997,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A79" sqref="A79"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8:H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1015,31 +1011,31 @@
     <col min="6" max="6" width="55" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="36.140625" customWidth="1"/>
     <col min="8" max="8" width="36.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="11.42578125" style="14"/>
+    <col min="9" max="16384" width="11.42578125" style="13"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13" t="s">
+      <c r="E1" s="12"/>
+      <c r="F1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="G1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="13" t="s">
-        <v>67</v>
+      <c r="H1" s="12" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -1053,13 +1049,13 @@
         <v>5</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F2" s="15" t="s">
-        <v>180</v>
-      </c>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
+        <v>25</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -1072,7 +1068,7 @@
         <v>7</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F3" t="s">
         <v>14</v>
@@ -1095,7 +1091,7 @@
         <v>10</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F4" t="s">
         <v>14</v>
@@ -1118,7 +1114,7 @@
         <v>13</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F5" t="s">
         <v>14</v>
@@ -1141,7 +1137,7 @@
         <v>17</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F6" t="s">
         <v>14</v>
@@ -1164,7 +1160,7 @@
         <v>22</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F7" t="s">
         <v>14</v>
@@ -1187,13 +1183,13 @@
         <v>23</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F8" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
+        <v>25</v>
+      </c>
+      <c r="F8" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -1203,19 +1199,19 @@
         <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F9" t="s">
         <v>26</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>27</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>28</v>
-      </c>
-      <c r="H9" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -1226,16 +1222,16 @@
         <v>3</v>
       </c>
       <c r="C10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F10" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="G10" s="15"/>
-      <c r="H10" s="15"/>
+        <v>25</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -1245,19 +1241,19 @@
         <v>3</v>
       </c>
       <c r="C11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F11" t="s">
         <v>26</v>
       </c>
-      <c r="F11" t="s">
-        <v>27</v>
-      </c>
       <c r="G11" t="s">
+        <v>29</v>
+      </c>
+      <c r="H11" t="s">
         <v>30</v>
-      </c>
-      <c r="H11" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -1268,16 +1264,16 @@
         <v>3</v>
       </c>
       <c r="C12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F12" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="G12" s="15"/>
-      <c r="H12" s="15"/>
+        <v>25</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -1287,19 +1283,19 @@
         <v>3</v>
       </c>
       <c r="C13" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F13" t="s">
+        <v>36</v>
+      </c>
+      <c r="G13" t="s">
         <v>35</v>
       </c>
-      <c r="E13" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F13" t="s">
-        <v>37</v>
-      </c>
-      <c r="G13" t="s">
-        <v>36</v>
-      </c>
       <c r="H13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -1310,19 +1306,19 @@
         <v>3</v>
       </c>
       <c r="C14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F14" t="s">
+        <v>36</v>
+      </c>
+      <c r="G14" t="s">
         <v>37</v>
       </c>
-      <c r="G14" t="s">
-        <v>38</v>
-      </c>
       <c r="H14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -1333,19 +1329,19 @@
         <v>3</v>
       </c>
       <c r="C15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G15" t="s">
+        <v>40</v>
+      </c>
+      <c r="H15" t="s">
         <v>41</v>
-      </c>
-      <c r="H15" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -1356,16 +1352,16 @@
         <v>3</v>
       </c>
       <c r="C16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F16" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="G16" s="15"/>
-      <c r="H16" s="15"/>
+        <v>25</v>
+      </c>
+      <c r="F16" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="G16" s="14"/>
+      <c r="H16" s="14"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
@@ -1375,16 +1371,16 @@
         <v>3</v>
       </c>
       <c r="C17" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F17" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="G17" s="15"/>
-      <c r="H17" s="15"/>
+        <v>25</v>
+      </c>
+      <c r="F17" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="G17" s="14"/>
+      <c r="H17" s="14"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
@@ -1394,16 +1390,16 @@
         <v>3</v>
       </c>
       <c r="C18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F18" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="G18" s="15"/>
-      <c r="H18" s="15"/>
+        <v>25</v>
+      </c>
+      <c r="F18" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="G18" s="14"/>
+      <c r="H18" s="14"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
@@ -1413,16 +1409,16 @@
         <v>3</v>
       </c>
       <c r="C19" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F19" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="G19" s="15"/>
-      <c r="H19" s="15"/>
+        <v>25</v>
+      </c>
+      <c r="F19" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="G19" s="14"/>
+      <c r="H19" s="14"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
@@ -1432,19 +1428,19 @@
         <v>3</v>
       </c>
       <c r="C20" t="s">
+        <v>48</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F20" t="s">
         <v>49</v>
       </c>
-      <c r="E20" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F20" t="s">
+      <c r="G20" t="s">
         <v>50</v>
       </c>
-      <c r="G20" t="s">
+      <c r="H20" t="s">
         <v>51</v>
-      </c>
-      <c r="H20" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -1455,16 +1451,16 @@
         <v>3</v>
       </c>
       <c r="C21" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F21" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="G21" s="15"/>
-      <c r="H21" s="15"/>
+        <v>25</v>
+      </c>
+      <c r="F21" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="G21" s="14"/>
+      <c r="H21" s="14"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
@@ -1474,16 +1470,16 @@
         <v>3</v>
       </c>
       <c r="C22" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F22" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="G22" s="15"/>
-      <c r="H22" s="15"/>
+        <v>25</v>
+      </c>
+      <c r="F22" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="G22" s="14"/>
+      <c r="H22" s="14"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
@@ -1493,16 +1489,16 @@
         <v>3</v>
       </c>
       <c r="C23" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F23" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="G23" s="15"/>
-      <c r="H23" s="15"/>
+        <v>25</v>
+      </c>
+      <c r="F23" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="G23" s="14"/>
+      <c r="H23" s="14"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
@@ -1512,16 +1508,16 @@
         <v>3</v>
       </c>
       <c r="C24" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F24" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="G24" s="15"/>
-      <c r="H24" s="15"/>
+        <v>25</v>
+      </c>
+      <c r="F24" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="G24" s="14"/>
+      <c r="H24" s="14"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
@@ -1531,19 +1527,19 @@
         <v>3</v>
       </c>
       <c r="C25" t="s">
+        <v>56</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F25" t="s">
+        <v>58</v>
+      </c>
+      <c r="G25" t="s">
         <v>57</v>
       </c>
-      <c r="E25" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F25" t="s">
+      <c r="H25" t="s">
         <v>59</v>
-      </c>
-      <c r="G25" t="s">
-        <v>58</v>
-      </c>
-      <c r="H25" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -1551,47 +1547,47 @@
         <v>1</v>
       </c>
       <c r="B26" t="s">
+        <v>76</v>
+      </c>
+      <c r="C26" t="s">
         <v>77</v>
       </c>
-      <c r="C26" t="s">
+      <c r="D26" t="s">
         <v>78</v>
       </c>
-      <c r="D26" t="s">
+      <c r="E26" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F26" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="E26" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F26" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="G26" s="12"/>
-      <c r="H26" s="12"/>
+      <c r="G26" s="15"/>
+      <c r="H26" s="15"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>1</v>
       </c>
       <c r="B27" t="s">
+        <v>76</v>
+      </c>
+      <c r="C27" t="s">
         <v>77</v>
       </c>
-      <c r="C27" t="s">
-        <v>78</v>
-      </c>
       <c r="D27" t="s">
+        <v>80</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F27" t="s">
         <v>81</v>
       </c>
-      <c r="E27" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F27" t="s">
+      <c r="G27" t="s">
         <v>82</v>
       </c>
-      <c r="G27" t="s">
+      <c r="H27" t="s">
         <v>83</v>
-      </c>
-      <c r="H27" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -1599,25 +1595,25 @@
         <v>1</v>
       </c>
       <c r="B28" t="s">
+        <v>76</v>
+      </c>
+      <c r="C28" t="s">
         <v>77</v>
       </c>
-      <c r="C28" t="s">
-        <v>78</v>
-      </c>
       <c r="D28" t="s">
+        <v>84</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F28" t="s">
         <v>85</v>
       </c>
-      <c r="E28" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F28" t="s">
+      <c r="G28" t="s">
         <v>86</v>
       </c>
-      <c r="G28" t="s">
-        <v>87</v>
-      </c>
       <c r="H28" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -1625,44 +1621,44 @@
         <v>1</v>
       </c>
       <c r="B29" t="s">
+        <v>76</v>
+      </c>
+      <c r="C29" t="s">
         <v>77</v>
       </c>
-      <c r="C29" t="s">
-        <v>78</v>
-      </c>
       <c r="D29" t="s">
+        <v>87</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F29" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="E29" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F29" s="15" t="s">
-        <v>89</v>
-      </c>
-      <c r="G29" s="15"/>
-      <c r="H29" s="15"/>
+      <c r="G29" s="14"/>
+      <c r="H29" s="14"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>1</v>
       </c>
       <c r="B30" t="s">
+        <v>76</v>
+      </c>
+      <c r="C30" t="s">
         <v>77</v>
       </c>
-      <c r="C30" t="s">
-        <v>78</v>
-      </c>
       <c r="D30" t="s">
+        <v>89</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F30" t="s">
+        <v>85</v>
+      </c>
+      <c r="G30" t="s">
         <v>90</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F30" t="s">
-        <v>86</v>
-      </c>
-      <c r="G30" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -1670,44 +1666,44 @@
         <v>1</v>
       </c>
       <c r="B31" t="s">
+        <v>76</v>
+      </c>
+      <c r="C31" t="s">
         <v>77</v>
       </c>
-      <c r="C31" t="s">
-        <v>78</v>
-      </c>
       <c r="D31" t="s">
+        <v>91</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F31" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="E31" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F31" s="12" t="s">
-        <v>93</v>
-      </c>
-      <c r="G31" s="12"/>
-      <c r="H31" s="12"/>
+      <c r="G31" s="15"/>
+      <c r="H31" s="15"/>
     </row>
     <row r="32" spans="1:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B32" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C32" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="C32" s="2" t="s">
-        <v>78</v>
-      </c>
       <c r="D32" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F32" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="E32" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F32" s="4" t="s">
+      <c r="G32" s="4" t="s">
         <v>95</v>
-      </c>
-      <c r="G32" s="4" t="s">
-        <v>96</v>
       </c>
       <c r="H32" s="2"/>
     </row>
@@ -1716,25 +1712,25 @@
         <v>1</v>
       </c>
       <c r="B33" t="s">
+        <v>76</v>
+      </c>
+      <c r="C33" t="s">
         <v>77</v>
       </c>
-      <c r="C33" t="s">
-        <v>78</v>
-      </c>
       <c r="D33" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F33" t="s">
+        <v>81</v>
+      </c>
+      <c r="G33" t="s">
         <v>82</v>
       </c>
-      <c r="G33" t="s">
+      <c r="H33" t="s">
         <v>83</v>
-      </c>
-      <c r="H33" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -1742,44 +1738,44 @@
         <v>1</v>
       </c>
       <c r="B34" t="s">
+        <v>76</v>
+      </c>
+      <c r="C34" t="s">
         <v>77</v>
       </c>
-      <c r="C34" t="s">
-        <v>78</v>
-      </c>
       <c r="D34" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F34" s="15" t="s">
-        <v>89</v>
-      </c>
-      <c r="G34" s="15"/>
-      <c r="H34" s="15"/>
+        <v>25</v>
+      </c>
+      <c r="F34" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="G34" s="14"/>
+      <c r="H34" s="14"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>1</v>
       </c>
       <c r="B35" t="s">
+        <v>76</v>
+      </c>
+      <c r="C35" t="s">
         <v>77</v>
       </c>
-      <c r="C35" t="s">
-        <v>78</v>
-      </c>
       <c r="D35" t="s">
+        <v>98</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F35" t="s">
         <v>99</v>
       </c>
-      <c r="E35" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F35" t="s">
+      <c r="G35" t="s">
         <v>100</v>
-      </c>
-      <c r="G35" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
@@ -1787,22 +1783,22 @@
         <v>1</v>
       </c>
       <c r="B36" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C36" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F36" t="s">
+        <v>104</v>
+      </c>
+      <c r="G36" t="s">
         <v>105</v>
       </c>
-      <c r="G36" t="s">
+      <c r="H36" t="s">
         <v>106</v>
-      </c>
-      <c r="H36" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
@@ -1810,19 +1806,19 @@
         <v>1</v>
       </c>
       <c r="B37" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C37" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F37" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G37" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
@@ -1830,19 +1826,19 @@
         <v>1</v>
       </c>
       <c r="B38" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C38" t="s">
+        <v>107</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F38" t="s">
         <v>108</v>
       </c>
-      <c r="E38" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F38" t="s">
-        <v>109</v>
-      </c>
       <c r="G38" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
@@ -1850,19 +1846,19 @@
         <v>1</v>
       </c>
       <c r="B39" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C39" t="s">
+        <v>109</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F39" t="s">
         <v>110</v>
       </c>
-      <c r="E39" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F39" t="s">
+      <c r="G39" t="s">
         <v>111</v>
-      </c>
-      <c r="G39" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
@@ -1870,19 +1866,19 @@
         <v>1</v>
       </c>
       <c r="B40" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C40" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F40" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G40" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
@@ -1890,22 +1886,22 @@
         <v>1</v>
       </c>
       <c r="B41" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C41" t="s">
+        <v>113</v>
+      </c>
+      <c r="D41" t="s">
         <v>114</v>
       </c>
-      <c r="D41" t="s">
+      <c r="E41" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F41" t="s">
+        <v>110</v>
+      </c>
+      <c r="G41" t="s">
         <v>115</v>
-      </c>
-      <c r="E41" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F41" t="s">
-        <v>111</v>
-      </c>
-      <c r="G41" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
@@ -1913,19 +1909,19 @@
         <v>1</v>
       </c>
       <c r="B42" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C42" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F42" t="s">
+        <v>116</v>
+      </c>
+      <c r="G42" t="s">
         <v>117</v>
-      </c>
-      <c r="G42" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
@@ -1933,19 +1929,19 @@
         <v>1</v>
       </c>
       <c r="B43" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C43" t="s">
+        <v>118</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F43" t="s">
         <v>119</v>
       </c>
-      <c r="E43" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F43" t="s">
+      <c r="G43" t="s">
         <v>120</v>
-      </c>
-      <c r="G43" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
@@ -1953,19 +1949,19 @@
         <v>1</v>
       </c>
       <c r="B44" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C44" t="s">
+        <v>121</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F44" t="s">
         <v>122</v>
       </c>
-      <c r="E44" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F44" t="s">
+      <c r="G44" t="s">
         <v>123</v>
-      </c>
-      <c r="G44" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
@@ -1973,19 +1969,19 @@
         <v>1</v>
       </c>
       <c r="B45" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C45" t="s">
+        <v>124</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F45" t="s">
+        <v>122</v>
+      </c>
+      <c r="G45" t="s">
         <v>125</v>
-      </c>
-      <c r="E45" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F45" t="s">
-        <v>123</v>
-      </c>
-      <c r="G45" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
@@ -1993,25 +1989,25 @@
         <v>1</v>
       </c>
       <c r="B46" t="s">
+        <v>61</v>
+      </c>
+      <c r="C46" t="s">
+        <v>60</v>
+      </c>
+      <c r="D46" t="s">
         <v>62</v>
       </c>
-      <c r="C46" t="s">
-        <v>61</v>
-      </c>
-      <c r="D46" t="s">
+      <c r="E46" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F46" t="s">
         <v>63</v>
       </c>
-      <c r="E46" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F46" t="s">
+      <c r="G46" t="s">
         <v>64</v>
       </c>
-      <c r="G46" t="s">
+      <c r="H46" t="s">
         <v>65</v>
-      </c>
-      <c r="H46" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
@@ -2019,25 +2015,25 @@
         <v>1</v>
       </c>
       <c r="B47" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C47" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D47" t="s">
+        <v>67</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F47" t="s">
+        <v>63</v>
+      </c>
+      <c r="G47" t="s">
         <v>68</v>
       </c>
-      <c r="E47" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F47" t="s">
-        <v>64</v>
-      </c>
-      <c r="G47" t="s">
+      <c r="H47" t="s">
         <v>69</v>
-      </c>
-      <c r="H47" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
@@ -2045,25 +2041,25 @@
         <v>1</v>
       </c>
       <c r="B48" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C48" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D48" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F48" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G48" t="s">
+        <v>72</v>
+      </c>
+      <c r="H48" t="s">
         <v>73</v>
-      </c>
-      <c r="H48" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
@@ -2071,25 +2067,25 @@
         <v>1</v>
       </c>
       <c r="B49" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C49" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D49" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F49" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G49" t="s">
+        <v>74</v>
+      </c>
+      <c r="H49" t="s">
         <v>75</v>
-      </c>
-      <c r="H49" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
@@ -2097,25 +2093,25 @@
         <v>1</v>
       </c>
       <c r="B50" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C50" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D50" t="s">
+        <v>138</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F50" t="s">
+        <v>63</v>
+      </c>
+      <c r="G50" t="s">
         <v>139</v>
       </c>
-      <c r="E50" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F50" t="s">
-        <v>64</v>
-      </c>
-      <c r="G50" t="s">
+      <c r="H50" t="s">
         <v>140</v>
-      </c>
-      <c r="H50" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
@@ -2123,25 +2119,25 @@
         <v>1</v>
       </c>
       <c r="B51" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C51" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D51" t="s">
+        <v>141</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F51" t="s">
+        <v>63</v>
+      </c>
+      <c r="G51" t="s">
         <v>142</v>
       </c>
-      <c r="E51" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F51" t="s">
-        <v>64</v>
-      </c>
-      <c r="G51" t="s">
+      <c r="H51" t="s">
         <v>143</v>
-      </c>
-      <c r="H51" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
@@ -2149,25 +2145,25 @@
         <v>1</v>
       </c>
       <c r="B52" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C52" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D52" t="s">
+        <v>144</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F52" t="s">
+        <v>63</v>
+      </c>
+      <c r="G52" t="s">
         <v>145</v>
       </c>
-      <c r="E52" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F52" t="s">
-        <v>64</v>
-      </c>
-      <c r="G52" t="s">
+      <c r="H52" t="s">
         <v>146</v>
-      </c>
-      <c r="H52" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
@@ -2175,22 +2171,22 @@
         <v>1</v>
       </c>
       <c r="B53" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C53" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F53" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G53" t="s">
+        <v>147</v>
+      </c>
+      <c r="H53" t="s">
         <v>148</v>
-      </c>
-      <c r="H53" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
@@ -2198,22 +2194,22 @@
         <v>1</v>
       </c>
       <c r="B54" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C54" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F54" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G54" t="s">
+        <v>139</v>
+      </c>
+      <c r="H54" t="s">
         <v>140</v>
-      </c>
-      <c r="H54" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
@@ -2221,41 +2217,41 @@
         <v>1</v>
       </c>
       <c r="B55" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C55" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F55" s="15" t="s">
-        <v>180</v>
-      </c>
-      <c r="G55" s="15"/>
-      <c r="H55" s="15"/>
+        <v>25</v>
+      </c>
+      <c r="F55" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="G55" s="14"/>
+      <c r="H55" s="14"/>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>1</v>
       </c>
       <c r="B56" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C56" t="s">
+        <v>127</v>
+      </c>
+      <c r="D56" t="s">
         <v>128</v>
       </c>
-      <c r="D56" t="s">
+      <c r="E56" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F56" t="s">
         <v>129</v>
       </c>
-      <c r="E56" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F56" t="s">
+      <c r="G56" t="s">
         <v>130</v>
-      </c>
-      <c r="G56" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="57" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -2263,22 +2259,22 @@
         <v>1</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D57" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="E57" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F57" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="E57" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F57" s="2" t="s">
+      <c r="G57" s="5" t="s">
         <v>133</v>
-      </c>
-      <c r="G57" s="5" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
@@ -2286,19 +2282,19 @@
         <v>1</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C58" t="s">
+        <v>134</v>
+      </c>
+      <c r="E58" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F58" t="s">
+        <v>129</v>
+      </c>
+      <c r="G58" t="s">
         <v>135</v>
-      </c>
-      <c r="E58" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F58" t="s">
-        <v>130</v>
-      </c>
-      <c r="G58" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
@@ -2306,19 +2302,19 @@
         <v>1</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C59" t="s">
+        <v>136</v>
+      </c>
+      <c r="E59" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F59" t="s">
+        <v>129</v>
+      </c>
+      <c r="G59" t="s">
         <v>137</v>
-      </c>
-      <c r="E59" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F59" t="s">
-        <v>130</v>
-      </c>
-      <c r="G59" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
@@ -2326,22 +2322,22 @@
         <v>1</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C60" t="s">
+        <v>150</v>
+      </c>
+      <c r="D60" t="s">
+        <v>128</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F60" t="s">
+        <v>129</v>
+      </c>
+      <c r="G60" t="s">
         <v>151</v>
-      </c>
-      <c r="D60" t="s">
-        <v>129</v>
-      </c>
-      <c r="E60" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F60" t="s">
-        <v>130</v>
-      </c>
-      <c r="G60" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="61" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -2349,22 +2345,22 @@
         <v>1</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D61" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F61" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="E61" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F61" s="2" t="s">
-        <v>133</v>
-      </c>
       <c r="G61" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
@@ -2372,39 +2368,39 @@
         <v>1</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C62" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F62" s="15" t="s">
-        <v>180</v>
-      </c>
-      <c r="G62" s="15"/>
-      <c r="H62" s="15"/>
+        <v>25</v>
+      </c>
+      <c r="F62" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="G62" s="14"/>
+      <c r="H62" s="14"/>
     </row>
     <row r="63" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D63" s="2"/>
       <c r="E63" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F63" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G63" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
@@ -2412,14 +2408,14 @@
         <v>1</v>
       </c>
       <c r="B64" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C64" s="7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D64" s="7"/>
       <c r="E64" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F64" s="7"/>
       <c r="G64" s="7"/>
@@ -2430,22 +2426,22 @@
         <v>1</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C65" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="E65" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F65" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G65" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="H65" s="5" t="s">
         <v>160</v>
-      </c>
-      <c r="E65" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F65" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="G65" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="H65" s="5" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
@@ -2453,14 +2449,14 @@
         <v>1</v>
       </c>
       <c r="B66" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C66" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D66" s="7"/>
       <c r="E66" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F66" s="7"/>
       <c r="G66" s="7"/>
@@ -2471,14 +2467,14 @@
         <v>1</v>
       </c>
       <c r="B67" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C67" s="7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D67" s="7"/>
       <c r="E67" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F67" s="7"/>
       <c r="G67" s="7"/>
@@ -2489,14 +2485,14 @@
         <v>1</v>
       </c>
       <c r="B68" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C68" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D68" s="7"/>
       <c r="E68" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F68" s="7"/>
       <c r="G68" s="7"/>
@@ -2507,14 +2503,14 @@
         <v>1</v>
       </c>
       <c r="B69" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C69" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D69" s="7"/>
       <c r="E69" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F69" s="7"/>
       <c r="G69" s="7"/>
@@ -2525,14 +2521,14 @@
         <v>1</v>
       </c>
       <c r="B70" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C70" s="7" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D70" s="7"/>
       <c r="E70" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F70" s="7"/>
       <c r="G70" s="7"/>
@@ -2543,58 +2539,58 @@
         <v>1</v>
       </c>
       <c r="B71" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C71" s="10" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D71" s="10"/>
       <c r="E71" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="F71" s="15" t="s">
-        <v>180</v>
-      </c>
-      <c r="G71" s="15"/>
-      <c r="H71" s="15"/>
+        <v>25</v>
+      </c>
+      <c r="F71" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="G71" s="14"/>
+      <c r="H71" s="14"/>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="9" t="s">
         <v>1</v>
       </c>
       <c r="B72" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C72" s="10" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D72" s="10"/>
       <c r="E72" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="F72" s="15" t="s">
-        <v>181</v>
-      </c>
-      <c r="G72" s="15"/>
-      <c r="H72" s="15"/>
+        <v>25</v>
+      </c>
+      <c r="F72" s="14" t="s">
+        <v>180</v>
+      </c>
+      <c r="G72" s="14"/>
+      <c r="H72" s="14"/>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="9" t="s">
         <v>1</v>
       </c>
       <c r="B73" s="9" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C73" s="10"/>
       <c r="D73" s="10"/>
       <c r="E73" s="11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F73" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="G73" s="10" t="s">
         <v>170</v>
-      </c>
-      <c r="G73" s="10" t="s">
-        <v>171</v>
       </c>
       <c r="H73" s="10"/>
     </row>
@@ -2603,22 +2599,22 @@
         <v>1</v>
       </c>
       <c r="B74" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="C74" t="s">
         <v>172</v>
       </c>
-      <c r="C74" t="s">
+      <c r="E74" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="F74" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="E74" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="F74" s="2" t="s">
+      <c r="G74" t="s">
+        <v>182</v>
+      </c>
+      <c r="H74" t="s">
         <v>174</v>
-      </c>
-      <c r="G74" t="s">
-        <v>183</v>
-      </c>
-      <c r="H74" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="75" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -2626,23 +2622,23 @@
         <v>1</v>
       </c>
       <c r="B75" s="9" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D75" s="2"/>
       <c r="E75" s="11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G75" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="H75" s="5" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
@@ -2650,22 +2646,22 @@
         <v>1</v>
       </c>
       <c r="B76" s="9" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E76" s="11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G76" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="H76" s="5" t="s">
         <v>183</v>
-      </c>
-      <c r="H76" s="5" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
@@ -2673,46 +2669,56 @@
         <v>1</v>
       </c>
       <c r="B77" s="9" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E77" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="F77" s="15" t="s">
-        <v>180</v>
-      </c>
-      <c r="G77" s="15"/>
-      <c r="H77" s="15"/>
+        <v>25</v>
+      </c>
+      <c r="F77" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="G77" s="14"/>
+      <c r="H77" s="14"/>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="9" t="s">
         <v>1</v>
       </c>
       <c r="B78" s="9" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E78" s="11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G78" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="H78" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:H1"/>
   <mergeCells count="21">
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="F8:H8"/>
+    <mergeCell ref="F10:H10"/>
+    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="F17:H17"/>
+    <mergeCell ref="F18:H18"/>
+    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="F21:H21"/>
+    <mergeCell ref="F22:H22"/>
     <mergeCell ref="F77:H77"/>
     <mergeCell ref="F23:H23"/>
     <mergeCell ref="F55:H55"/>
@@ -2724,16 +2730,6 @@
     <mergeCell ref="F31:H31"/>
     <mergeCell ref="F34:H34"/>
     <mergeCell ref="F24:H24"/>
-    <mergeCell ref="F17:H17"/>
-    <mergeCell ref="F18:H18"/>
-    <mergeCell ref="F19:H19"/>
-    <mergeCell ref="F21:H21"/>
-    <mergeCell ref="F22:H22"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="F8:H8"/>
-    <mergeCell ref="F10:H10"/>
-    <mergeCell ref="F12:H12"/>
-    <mergeCell ref="F16:H16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>